<commit_message>
Mudei isto e aquilo.
</commit_message>
<xml_diff>
--- a/Docs/Test Results/usability_kevin.xlsx
+++ b/Docs/Test Results/usability_kevin.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dropbox\ISEC\MIS\1º ANO\Projecto de Software\Repository\Docs\Test Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\João\Documents\Aulas\Mestrado\Projeto Software\Docs\Test Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>Add task</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>foi logo aos settings. Fechou a janela porque não conseguiu alterar o tempo (CHECKBOX!!!) e depois foi editar tarefa. Voltou aos settings e activou a check.  Disparou logo o alerta mal fez play na tarefa. Disparou sem parar e criou frustração.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -186,8 +189,8 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Correto" xfId="1" builtinId="26"/>
-    <cellStyle name="Incorreto" xfId="2" builtinId="27"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -204,7 +207,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -469,17 +472,17 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C21" sqref="C20:C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="58.42578125" customWidth="1"/>
+    <col min="1" max="1" width="26.109375" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="58.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>19</v>
       </c>
@@ -493,7 +496,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -507,7 +510,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -521,7 +524,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -535,7 +538,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -549,7 +552,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -563,7 +566,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -577,7 +580,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -591,7 +594,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -605,7 +608,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -619,7 +622,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>9</v>
       </c>
@@ -631,7 +634,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C13" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>22</v>
       </c>

</xml_diff>